<commit_message>
add vendor support for huawei router
</commit_message>
<xml_diff>
--- a/mop_db.xlsx
+++ b/mop_db.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akrommusajid/MyProject/scriptmaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5BF82A-C459-BC49-B64A-4034C9D1099A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F2CF6E-C29C-2445-A694-881F04F82FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="3" xr2:uid="{1C3DAC1A-8410-4843-8D0A-26CD0BB45E0E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{1C3DAC1A-8410-4843-8D0A-26CD0BB45E0E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="portchannel" sheetId="9" r:id="rId1"/>
     <sheet name="integration" sheetId="1" r:id="rId2"/>
-    <sheet name="ospf" sheetId="2" r:id="rId3"/>
-    <sheet name="port_migration" sheetId="8" r:id="rId4"/>
-    <sheet name="bgp_as_consolidation" sheetId="5" r:id="rId5"/>
-    <sheet name="vrf" sheetId="7" r:id="rId6"/>
-    <sheet name="bfd" sheetId="6" r:id="rId7"/>
+    <sheet name="static" sheetId="10" r:id="rId3"/>
+    <sheet name="ospf" sheetId="2" r:id="rId4"/>
+    <sheet name="port_migration" sheetId="8" r:id="rId5"/>
+    <sheet name="bgp_as_consolidation" sheetId="5" r:id="rId6"/>
+    <sheet name="vrf" sheetId="7" r:id="rId7"/>
     <sheet name="bgp" sheetId="3" r:id="rId8"/>
+    <sheet name="bfd" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
   <si>
     <t>node_A</t>
   </si>
@@ -97,9 +98,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>Global</t>
   </si>
   <si>
     <t>bridge_domain</t>
@@ -388,6 +386,72 @@
   </si>
   <si>
     <t>router-surabaya</t>
+  </si>
+  <si>
+    <t>GigabitEthernet5/0/7</t>
+  </si>
+  <si>
+    <t>huawei</t>
+  </si>
+  <si>
+    <t>node_B_portchannel</t>
+  </si>
+  <si>
+    <t>node_B_vendor</t>
+  </si>
+  <si>
+    <t>node_A_portchannel</t>
+  </si>
+  <si>
+    <t>node_A_vendor</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>nexthop</t>
+  </si>
+  <si>
+    <t>10.14.25.18</t>
+  </si>
+  <si>
+    <t>255.255.255.255</t>
+  </si>
+  <si>
+    <t>10.254.17.197</t>
+  </si>
+  <si>
+    <t>10.14.25.19</t>
+  </si>
+  <si>
+    <t>10.14.25.20</t>
+  </si>
+  <si>
+    <t>Te1/1/5</t>
+  </si>
+  <si>
+    <t>ldp</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>to_Madiun</t>
+  </si>
+  <si>
+    <t>router_bogor</t>
+  </si>
+  <si>
+    <t>router_madiun</t>
+  </si>
+  <si>
+    <t>auth</t>
+  </si>
+  <si>
+    <t>global</t>
   </si>
 </sst>
 </file>
@@ -435,10 +499,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -754,23 +822,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901E0C69-5F2B-8945-8568-ED214A2E7D88}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356785D0-A3B3-6445-8D7A-4F2B4B1A4C82}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACC5748-B99B-9F44-A2F1-D3A6D5B4A619}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,48 +949,60 @@
     <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -841,6 +1012,121 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D99100-26D8-E54E-B55C-52D296B31415}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646E889B-9F9D-F346-8E32-CBD376A25C4C}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -880,7 +1166,7 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -888,11 +1174,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133F7934-EE35-044A-BE38-2611281E3093}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -910,110 +1196,110 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="221" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="238" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="372" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="388" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="356" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1022,12 +1308,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8CF646-1BF0-AD47-A7C0-64B5A402C878}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,113 +1322,115 @@
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.1640625" customWidth="1"/>
     <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="D2">
+        <v>65102</v>
+      </c>
+      <c r="E2">
+        <v>65001</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>65102</v>
+      </c>
+      <c r="E3">
+        <v>65001</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2">
-        <v>65102</v>
-      </c>
-      <c r="D2">
-        <v>65001</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3">
-        <v>65102</v>
-      </c>
-      <c r="D3">
-        <v>65001</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1150,7 +1438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6275434-5C14-194D-9B1C-D23C85002DFB}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1160,111 +1448,111 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1560,122 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED83FF2-7059-664F-A171-B6DC254C01F9}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>65102</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2">
+        <v>65001</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>65102</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3">
+        <v>65001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D54A82-839F-E446-A92B-A985C8BD8DB3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1284,110 +1687,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED83FF2-7059-664F-A171-B6DC254C01F9}">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2">
-        <v>65102</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2">
-        <v>65001</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3">
-        <v>65102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3">
-        <v>65001</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>